<commit_message>
corrected coding logic mistake
</commit_message>
<xml_diff>
--- a/TEST/Setup.xlsx
+++ b/TEST/Setup.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CD0723EE-DEE1-4CFC-B81C-5373A16D1A86}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0CAAB333-3C61-4079-BB88-43516FE48D49}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="18">
   <si>
     <t>Pair</t>
   </si>
@@ -43,34 +43,37 @@
     <t>EURJPY</t>
   </si>
   <si>
-    <t>GBPCHF</t>
-  </si>
-  <si>
-    <t>CADJPY</t>
-  </si>
-  <si>
-    <t>GBPJPY</t>
-  </si>
-  <si>
-    <t>AUDNZD</t>
-  </si>
-  <si>
-    <t>AUDCAD</t>
-  </si>
-  <si>
-    <t>AUDCHF</t>
-  </si>
-  <si>
-    <t>AUDJPY</t>
-  </si>
-  <si>
-    <t>CHFJPY</t>
-  </si>
-  <si>
-    <t>EURNZD</t>
-  </si>
-  <si>
-    <t>EURCAD</t>
+    <t>USDCHF</t>
+  </si>
+  <si>
+    <t>GBPUSD</t>
+  </si>
+  <si>
+    <t>EURUSD</t>
+  </si>
+  <si>
+    <t>USDJPY</t>
+  </si>
+  <si>
+    <t>USDCAD</t>
+  </si>
+  <si>
+    <t>AUDUSD</t>
+  </si>
+  <si>
+    <t>EURGBP</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>scalper</t>
+  </si>
+  <si>
+    <t>daily</t>
+  </si>
+  <si>
+    <t>longterm</t>
   </si>
 </sst>
 </file>
@@ -388,15 +391,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -406,148 +409,428 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>8137401</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>8137402</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>8137403</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>8137404</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>8137405</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>8137406</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>8137407</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>8138401</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>8137408</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>8138402</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>8137409</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>8138403</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>8137410</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>8138410</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>8137411</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>8138411</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>8137412</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7">
-        <v>8138412</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>8137413</v>
+      </c>
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8">
-        <v>8138420</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>8137414</v>
+      </c>
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9">
-        <v>8138421</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>8137415</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>12</v>
       </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10">
-        <v>8138422</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>8137416</v>
+      </c>
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>13</v>
       </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11">
-        <v>8138423</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12">
-        <v>8138413</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13">
-        <v>8138414</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14">
-        <v>8138415</v>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>8137417</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>8137418</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>8137419</v>
+      </c>
+      <c r="D20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <v>8137420</v>
+      </c>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>8137421</v>
+      </c>
+      <c r="D22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>8137422</v>
+      </c>
+      <c r="D23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24">
+        <v>8137423</v>
+      </c>
+      <c r="D24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <v>8137424</v>
+      </c>
+      <c r="D25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26">
+        <v>8137425</v>
+      </c>
+      <c r="D26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>8137426</v>
+      </c>
+      <c r="D27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>8137427</v>
+      </c>
+      <c r="D28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>8137428</v>
+      </c>
+      <c r="D29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>8137429</v>
+      </c>
+      <c r="D30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31">
+        <v>8137430</v>
+      </c>
+      <c r="D31" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>